<commit_message>
Fixed double counting and missing sectors in processing REAS data ( E.REAS_emissions.R ). Updated REAS related scaling mapping files.
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/REAS_scaling_mapping_AgrWaste.xlsx
+++ b/input/mappings/scaling/REAS_scaling_mapping_AgrWaste.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="0" windowWidth="16920" windowHeight="13960" tabRatio="500"/>
+    <workbookView xWindow="900" yWindow="0" windowWidth="16920" windowHeight="13620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
@@ -12,16 +12,11 @@
     <sheet name="year" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
   <si>
     <t>pre_ext_method</t>
   </si>
@@ -86,15 +81,6 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>rice_cultivation</t>
-  </si>
-  <si>
-    <t>manure_management</t>
-  </si>
-  <si>
-    <t>enteric_fermentati</t>
-  </si>
-  <si>
     <t>enteric-fermentation</t>
   </si>
   <si>
@@ -104,12 +90,6 @@
     <t>rice-cultivation</t>
   </si>
   <si>
-    <t>urea</t>
-  </si>
-  <si>
-    <t>fertilizer</t>
-  </si>
-  <si>
     <t>soil-emissions</t>
   </si>
   <si>
@@ -119,19 +99,51 @@
     <t>solid_waste</t>
   </si>
   <si>
-    <t>waste</t>
-  </si>
-  <si>
-    <t>human</t>
+    <t>ncomb-agriculture-manure_management</t>
+  </si>
+  <si>
+    <t>ncomb-industry-urea</t>
+  </si>
+  <si>
+    <t>ncomb-agriculture-fertilizer</t>
+  </si>
+  <si>
+    <t>ncomb-others-waste_water</t>
+  </si>
+  <si>
+    <t>ncomb-others-human</t>
+  </si>
+  <si>
+    <t>ncomb-agriculture-enteric_fermentati</t>
+  </si>
+  <si>
+    <t>ncomb-agriculture-rice_cultivation</t>
+  </si>
+  <si>
+    <t>ncomb-others-waste</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -159,16 +171,316 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -176,578 +488,765 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="563">
+  <cellStyleXfs count="606">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="603"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="603"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="603"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="603"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="605"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="603" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="605"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="605"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="563">
+  <cellStyles count="606">
+    <cellStyle name="20% - Accent1" xfId="580" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="584" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="588" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="592" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="596" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="600" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="581" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="585" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="589" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="593" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="597" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="601" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="582" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="586" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="590" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="594" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="598" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="602" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="579" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="583" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="587" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="591" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="595" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="599" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="569" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="573" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="575" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="577" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1029,6 +1528,11 @@
     <cellStyle name="Followed Hyperlink" xfId="558" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="560" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="562" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="568" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="564" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="565" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="566" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="567" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1310,10 +1814,25 @@
     <cellStyle name="Hyperlink" xfId="557" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="559" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="561" builtinId="8" hidden="1"/>
+    <cellStyle name="Input" xfId="571" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="574" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="570" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="603"/>
+    <cellStyle name="Normal 3" xfId="605"/>
+    <cellStyle name="Note 2" xfId="604"/>
+    <cellStyle name="Output" xfId="572" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="563" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="578" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="576" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1645,19 +2164,19 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A13" sqref="A13:XFD19"/>
+      <selection pane="bottomRight" activeCell="A10" sqref="A10:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="27.1640625" customWidth="1"/>
+    <col min="1" max="1" width="18.375" customWidth="1"/>
+    <col min="2" max="2" width="27.125" customWidth="1"/>
     <col min="3" max="3" width="26.5" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="7" max="7" width="26.6640625" customWidth="1"/>
+    <col min="7" max="7" width="26.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1671,103 +2190,103 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>23</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
         <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>21</v>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>27</v>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>28</v>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>32</v>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>31</v>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>33</v>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="4:4">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="4:4">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="2"/>
     </row>
   </sheetData>
@@ -1776,11 +2295,6 @@
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1792,14 +2306,14 @@
       <selection activeCell="D2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.875" customWidth="1"/>
+    <col min="5" max="5" width="13.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1816,7 +2330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1852,12 +2366,12 @@
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1883,7 +2397,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>

</xml_diff>